<commit_message>
Processo - Mover pasta
</commit_message>
<xml_diff>
--- a/config/E-mails para Notificações – RPA.xlsx
+++ b/config/E-mails para Notificações – RPA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RPA\compassEvaBuscaDeLivros\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1FE817A9-1E9D-4CF4-9B50-358062982913}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{581EC00B-9711-4351-A2D2-6C494A24BC17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-51600" yWindow="0" windowWidth="25800" windowHeight="21000" xr2:uid="{6B9D7671-F48A-43B2-A0E0-73424A4C293D}"/>
+    <workbookView xWindow="-41460" yWindow="4290" windowWidth="19575" windowHeight="15435" xr2:uid="{6B9D7671-F48A-43B2-A0E0-73424A4C293D}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -67,10 +67,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -96,8 +103,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32ED061C-E254-412C-A05B-E31E3D4B5BF4}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -424,7 +432,7 @@
     <col min="2" max="2" width="39.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -432,44 +440,42 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="I2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="I3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
+      <c r="I4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
+      <c r="I5" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Notificar finalização do processo e mover pasta
</commit_message>
<xml_diff>
--- a/config/E-mails para Notificações – RPA.xlsx
+++ b/config/E-mails para Notificações – RPA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RPA\compassEvaBuscaDeLivros\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1FE817A9-1E9D-4CF4-9B50-358062982913}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{008E7A98-33EB-48D6-82A9-DB2E439FBE7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-51600" yWindow="0" windowWidth="25800" windowHeight="21000" xr2:uid="{6B9D7671-F48A-43B2-A0E0-73424A4C293D}"/>
+    <workbookView xWindow="-51600" yWindow="2325" windowWidth="26715" windowHeight="15435" xr2:uid="{6B9D7671-F48A-43B2-A0E0-73424A4C293D}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -412,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32ED061C-E254-412C-A05B-E31E3D4B5BF4}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -424,7 +424,7 @@
     <col min="2" max="2" width="39.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -432,44 +432,44 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="O3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="O4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N5" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
+      <c r="O5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N6" t="s">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
+      <c r="O6" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>